<commit_message>
upgrade dfa summary function to calculate visit times diff
</commit_message>
<xml_diff>
--- a/Documents/Castor_validation.xlsx
+++ b/Documents/Castor_validation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="224">
   <si>
     <t>SubjectID</t>
   </si>
@@ -463,6 +463,9 @@
     <t>27-04-2023</t>
   </si>
   <si>
+    <t>27-07-2023</t>
+  </si>
+  <si>
     <t>08-05-2023</t>
   </si>
   <si>
@@ -508,6 +511,9 @@
     <t>18-08-2023</t>
   </si>
   <si>
+    <t>05-09-2023</t>
+  </si>
+  <si>
     <t>08-03-2023</t>
   </si>
   <si>
@@ -541,6 +547,9 @@
     <t>04-05-2023</t>
   </si>
   <si>
+    <t>02-08-2023</t>
+  </si>
+  <si>
     <t>24-07-2023</t>
   </si>
   <si>
@@ -568,6 +577,9 @@
     <t>14-07-2023</t>
   </si>
   <si>
+    <t>12-09-2023</t>
+  </si>
+  <si>
     <t>20-03-2023</t>
   </si>
   <si>
@@ -607,15 +619,21 @@
     <t>17-07-2023</t>
   </si>
   <si>
-    <t>02-08-2023</t>
-  </si>
-  <si>
     <t>11-04-2023</t>
   </si>
   <si>
+    <t>06-09-2023</t>
+  </si>
+  <si>
     <t>18-05-2023</t>
   </si>
   <si>
+    <t>08-09-2023</t>
+  </si>
+  <si>
+    <t>04-09-2023</t>
+  </si>
+  <si>
     <t>03-04-2023</t>
   </si>
   <si>
@@ -628,6 +646,15 @@
     <t>05-06-2023</t>
   </si>
   <si>
+    <t>13-09-2023</t>
+  </si>
+  <si>
+    <t>15-09-2023</t>
+  </si>
+  <si>
+    <t>14-09-2023</t>
+  </si>
+  <si>
     <t>31-03-2023</t>
   </si>
   <si>
@@ -635,6 +662,9 @@
   </si>
   <si>
     <t>26-06-2023</t>
+  </si>
+  <si>
+    <t>01-06-2023</t>
   </si>
   <si>
     <t>07-04-2023</t>
@@ -1097,13 +1127,13 @@
         <v>101</v>
       </c>
       <c r="F3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -1123,10 +1153,10 @@
         <v>102</v>
       </c>
       <c r="F4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G4" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1146,13 +1176,13 @@
         <v>103</v>
       </c>
       <c r="F5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G5" t="s">
         <v>140</v>
       </c>
       <c r="H5" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="I5" t="s">
         <v>108</v>
@@ -1175,10 +1205,10 @@
         <v>103</v>
       </c>
       <c r="F6" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G6" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1198,16 +1228,16 @@
         <v>104</v>
       </c>
       <c r="F7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G7" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="H7" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="I7" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="J7" t="s">
         <v>108</v>
@@ -1233,7 +1263,7 @@
         <v>146</v>
       </c>
       <c r="G8" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="H8" t="s">
         <v>108</v>
@@ -1307,7 +1337,19 @@
         <v>109</v>
       </c>
       <c r="F12" t="s">
-        <v>157</v>
+        <v>158</v>
+      </c>
+      <c r="G12" t="s">
+        <v>172</v>
+      </c>
+      <c r="H12" t="s">
+        <v>171</v>
+      </c>
+      <c r="I12" t="s">
+        <v>205</v>
+      </c>
+      <c r="J12" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -1327,22 +1369,22 @@
         <v>110</v>
       </c>
       <c r="F13" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G13" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H13" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="I13" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="J13" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="K13" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="L13" t="s">
         <v>140</v>
@@ -1354,10 +1396,10 @@
         <v>106</v>
       </c>
       <c r="O13" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="P13" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -1380,16 +1422,16 @@
         <v>101</v>
       </c>
       <c r="G14" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H14" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="I14" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="J14" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="K14" t="s">
         <v>140</v>
@@ -1415,10 +1457,10 @@
         <v>111</v>
       </c>
       <c r="F15" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G15" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -1438,10 +1480,10 @@
         <v>101</v>
       </c>
       <c r="F16" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G16" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -1467,7 +1509,7 @@
         <v>113</v>
       </c>
       <c r="H17" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I17" t="s">
         <v>127</v>
@@ -1504,10 +1546,10 @@
         <v>113</v>
       </c>
       <c r="F19" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G19" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -1533,31 +1575,31 @@
         <v>115</v>
       </c>
       <c r="H20" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I20" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="J20" t="s">
         <v>116</v>
       </c>
       <c r="K20" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="L20" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="M20" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="N20" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="O20" t="s">
         <v>133</v>
       </c>
       <c r="P20" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -1577,31 +1619,31 @@
         <v>115</v>
       </c>
       <c r="F21" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G21" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="H21" t="s">
         <v>116</v>
       </c>
       <c r="I21" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="J21" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="K21" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="L21" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="M21" t="s">
         <v>133</v>
       </c>
       <c r="N21" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -1638,13 +1680,19 @@
         <v>117</v>
       </c>
       <c r="F23" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G23" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="H23" t="s">
-        <v>189</v>
+        <v>193</v>
+      </c>
+      <c r="I23" t="s">
+        <v>165</v>
+      </c>
+      <c r="J23" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="24" spans="1:16">
@@ -1664,13 +1712,13 @@
         <v>118</v>
       </c>
       <c r="F24" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G24" t="s">
         <v>133</v>
       </c>
       <c r="H24" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="25" spans="1:16">
@@ -1689,6 +1737,12 @@
       <c r="E25" t="s">
         <v>119</v>
       </c>
+      <c r="F25" t="s">
+        <v>165</v>
+      </c>
+      <c r="G25" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="26" spans="1:16">
       <c r="A26" s="1">
@@ -1707,7 +1761,7 @@
         <v>120</v>
       </c>
       <c r="F26" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="G26" t="s">
         <v>102</v>
@@ -1716,13 +1770,13 @@
         <v>104</v>
       </c>
       <c r="I26" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="J26" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="K26" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="L26" t="s">
         <v>121</v>
@@ -1757,28 +1811,28 @@
         <v>120</v>
       </c>
       <c r="F27" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="G27" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="H27" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="I27" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="J27" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="K27" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="L27" t="s">
         <v>139</v>
       </c>
       <c r="M27" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="N27" t="s">
         <v>122</v>
@@ -1879,7 +1933,7 @@
         <v>106</v>
       </c>
       <c r="F31" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="G31" t="s">
         <v>127</v>
@@ -1908,28 +1962,28 @@
         <v>123</v>
       </c>
       <c r="F32" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="G32" t="s">
         <v>126</v>
       </c>
       <c r="H32" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="I32" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="J32" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="K32" t="s">
         <v>130</v>
       </c>
       <c r="L32" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
       <c r="M32" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="N32" t="s">
         <v>131</v>
@@ -1938,7 +1992,7 @@
         <v>109</v>
       </c>
       <c r="P32" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:14">
@@ -2022,7 +2076,7 @@
         <v>115</v>
       </c>
       <c r="I35" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="J35" t="s">
         <v>116</v>
@@ -2106,16 +2160,16 @@
         <v>129</v>
       </c>
       <c r="I38" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="J38" t="s">
         <v>130</v>
       </c>
       <c r="K38" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="L38" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="M38" t="s">
         <v>132</v>
@@ -2144,25 +2198,25 @@
         <v>129</v>
       </c>
       <c r="H39" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="I39" t="s">
         <v>130</v>
       </c>
       <c r="J39" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K39" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="L39" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="M39" t="s">
         <v>132</v>
       </c>
       <c r="N39" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="40" spans="1:14">
@@ -2202,16 +2256,16 @@
         <v>128</v>
       </c>
       <c r="F41" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G41" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="H41" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="I41" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="J41" t="s">
         <v>131</v>
@@ -2220,10 +2274,13 @@
         <v>109</v>
       </c>
       <c r="L41" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="M41" t="s">
-        <v>169</v>
+        <v>171</v>
+      </c>
+      <c r="N41" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="42" spans="1:14">
@@ -2243,7 +2300,7 @@
         <v>129</v>
       </c>
       <c r="F42" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="43" spans="1:14">
@@ -2263,22 +2320,25 @@
         <v>130</v>
       </c>
       <c r="F43" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G43" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H43" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="I43" t="s">
         <v>132</v>
       </c>
       <c r="J43" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="K43" t="s">
-        <v>186</v>
+        <v>190</v>
+      </c>
+      <c r="L43" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="44" spans="1:14">
@@ -2298,7 +2358,7 @@
         <v>131</v>
       </c>
       <c r="F44" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="45" spans="1:14">
@@ -2318,10 +2378,10 @@
         <v>109</v>
       </c>
       <c r="F45" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="G45" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="46" spans="1:14">
@@ -2341,13 +2401,13 @@
         <v>109</v>
       </c>
       <c r="F46" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G46" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="H46" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="47" spans="1:14">
@@ -2367,10 +2427,10 @@
         <v>132</v>
       </c>
       <c r="F47" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="G47" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="48" spans="1:14">
@@ -2390,7 +2450,7 @@
         <v>133</v>
       </c>
       <c r="F48" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="49" spans="1:16">
@@ -2450,10 +2510,10 @@
         <v>136</v>
       </c>
       <c r="H51" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="I51" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="52" spans="1:16">
@@ -2473,13 +2533,13 @@
         <v>135</v>
       </c>
       <c r="F52" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G52" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H52" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="I52" t="s">
         <v>112</v>
@@ -2528,31 +2588,31 @@
         <v>101</v>
       </c>
       <c r="G54" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H54" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I54" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="J54" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="K54" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="L54" t="s">
         <v>140</v>
       </c>
       <c r="M54" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="N54" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="O54" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="P54" t="s">
         <v>113</v>
@@ -2578,7 +2638,7 @@
         <v>136</v>
       </c>
       <c r="G55" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="H55" t="s">
         <v>103</v>
@@ -2604,7 +2664,7 @@
         <v>136</v>
       </c>
       <c r="G56" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="H56" t="s">
         <v>103</v>
@@ -2613,7 +2673,7 @@
         <v>105</v>
       </c>
       <c r="J56" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="57" spans="1:16">
@@ -2633,13 +2693,13 @@
         <v>101</v>
       </c>
       <c r="F57" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G57" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="H57" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="I57" t="s">
         <v>147</v>
@@ -2648,10 +2708,10 @@
         <v>112</v>
       </c>
       <c r="K57" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="L57" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="M57" t="s">
         <v>113</v>
@@ -2680,13 +2740,13 @@
         <v>147</v>
       </c>
       <c r="H58" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="I58" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="J58" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="59" spans="1:16">
@@ -2720,22 +2780,31 @@
         <v>139</v>
       </c>
       <c r="F60" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G60" t="s">
         <v>107</v>
       </c>
       <c r="H60" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="I60" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="J60" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="K60" t="s">
-        <v>201</v>
+        <v>207</v>
+      </c>
+      <c r="L60" t="s">
+        <v>215</v>
+      </c>
+      <c r="M60" t="s">
+        <v>130</v>
+      </c>
+      <c r="N60" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="61" spans="1:16">
@@ -2758,16 +2827,16 @@
         <v>112</v>
       </c>
       <c r="G61" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="H61" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="I61" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="J61" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
     </row>
     <row r="62" spans="1:16">
@@ -2787,16 +2856,16 @@
         <v>141</v>
       </c>
       <c r="F62" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G62" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H62" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="I62" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="63" spans="1:16">
@@ -2816,10 +2885,16 @@
         <v>142</v>
       </c>
       <c r="F63" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G63" t="s">
-        <v>189</v>
+        <v>193</v>
+      </c>
+      <c r="H63" t="s">
+        <v>165</v>
+      </c>
+      <c r="I63" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="64" spans="1:16">
@@ -2839,13 +2914,19 @@
         <v>127</v>
       </c>
       <c r="F64" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="G64" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10">
+        <v>153</v>
+      </c>
+      <c r="H64" t="s">
+        <v>202</v>
+      </c>
+      <c r="I64" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -2862,10 +2943,10 @@
         <v>141</v>
       </c>
       <c r="F65" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -2882,7 +2963,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:11">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -2902,7 +2983,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:11">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -2918,8 +2999,17 @@
       <c r="E68" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="69" spans="1:10">
+      <c r="F68" t="s">
+        <v>119</v>
+      </c>
+      <c r="G68" t="s">
+        <v>165</v>
+      </c>
+      <c r="H68" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -2942,7 +3032,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:11">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -2962,7 +3052,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:11">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -2982,19 +3072,22 @@
         <v>148</v>
       </c>
       <c r="G71" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="H71" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="I71" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="J71" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10">
+        <v>208</v>
+      </c>
+      <c r="K71" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -3011,27 +3104,42 @@
         <v>148</v>
       </c>
       <c r="F72" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="G72" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="H72" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10">
+        <v>203</v>
+      </c>
+      <c r="I72" t="s">
+        <v>208</v>
+      </c>
+      <c r="J72" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
       <c r="A73" s="1">
         <v>71</v>
       </c>
       <c r="B73" t="s">
         <v>86</v>
       </c>
+      <c r="C73" t="s">
+        <v>96</v>
+      </c>
       <c r="D73" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="74" spans="1:10">
+      <c r="E73" t="s">
+        <v>149</v>
+      </c>
+      <c r="F73" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -3045,13 +3153,13 @@
         <v>100</v>
       </c>
       <c r="E74" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F74" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:11">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -3071,10 +3179,10 @@
         <v>116</v>
       </c>
       <c r="G75" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -3088,16 +3196,16 @@
         <v>100</v>
       </c>
       <c r="E76" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F76" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="G76" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -3111,10 +3219,13 @@
         <v>100</v>
       </c>
       <c r="E77" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10">
+        <v>152</v>
+      </c>
+      <c r="F77" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -3128,16 +3239,22 @@
         <v>100</v>
       </c>
       <c r="E78" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F78" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="G78" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10">
+        <v>174</v>
+      </c>
+      <c r="H78" t="s">
+        <v>204</v>
+      </c>
+      <c r="I78" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -3154,7 +3271,16 @@
         <v>132</v>
       </c>
       <c r="F79" t="s">
-        <v>177</v>
+        <v>180</v>
+      </c>
+      <c r="G79" t="s">
+        <v>190</v>
+      </c>
+      <c r="H79" t="s">
+        <v>165</v>
+      </c>
+      <c r="I79" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>